<commit_message>
Modificacion Modelo y Run Instancias
</commit_message>
<xml_diff>
--- a/Data in/Base MicroHub.xlsx
+++ b/Data in/Base MicroHub.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Investigacion JC - PH\Data in\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7650"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -28,15 +36,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -47,38 +56,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -268,592 +284,597 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AU4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>1.4401537E8</v>
+        <v>144015370</v>
       </c>
       <c r="C1" s="1">
-        <v>1.83347E8</v>
+        <v>183347000</v>
       </c>
       <c r="D1" s="1">
-        <v>2.55805128E8</v>
+        <v>255805128</v>
       </c>
       <c r="E1" s="1">
-        <v>2.5580513E8</v>
+        <v>255805130</v>
       </c>
       <c r="F1" s="1">
-        <v>2.55805131E8</v>
+        <v>255805131</v>
       </c>
       <c r="G1" s="1">
-        <v>2.55805132E8</v>
+        <v>255805132</v>
       </c>
       <c r="H1" s="1">
-        <v>2.72112665E8</v>
+        <v>272112665</v>
       </c>
       <c r="I1" s="1">
-        <v>2.73273842E8</v>
+        <v>273273842</v>
       </c>
       <c r="J1" s="1">
-        <v>2.78048435E8</v>
+        <v>278048435</v>
       </c>
       <c r="K1" s="1">
-        <v>2.92333297E8</v>
+        <v>292333297</v>
       </c>
       <c r="L1" s="1">
-        <v>2.92333298E8</v>
+        <v>292333298</v>
       </c>
       <c r="M1" s="1">
-        <v>3.08975873E8</v>
+        <v>308975873</v>
       </c>
       <c r="N1" s="1">
-        <v>3.2043212E8</v>
+        <v>320432120</v>
       </c>
       <c r="O1" s="1">
-        <v>3.63025783E8</v>
+        <v>363025783</v>
       </c>
       <c r="P1" s="1">
-        <v>4.49580382E8</v>
+        <v>449580382</v>
       </c>
       <c r="Q1" s="1">
-        <v>5.08568769E8</v>
+        <v>508568769</v>
       </c>
       <c r="R1" s="1">
-        <v>5.21115611E8</v>
+        <v>521115611</v>
       </c>
       <c r="S1" s="1">
-        <v>5.42846155E8</v>
+        <v>542846155</v>
       </c>
       <c r="T1" s="1">
-        <v>5.49861589E8</v>
+        <v>549861589</v>
       </c>
       <c r="U1" s="1">
-        <v>5.51078716E8</v>
+        <v>551078716</v>
       </c>
       <c r="V1" s="1">
-        <v>5.51331548E8</v>
+        <v>551331548</v>
       </c>
       <c r="W1" s="1">
-        <v>5.55782222E8</v>
+        <v>555782222</v>
       </c>
       <c r="X1" s="1">
-        <v>5.78703831E8</v>
+        <v>578703831</v>
       </c>
       <c r="Y1" s="1">
-        <v>5.78703832E8</v>
+        <v>578703832</v>
       </c>
       <c r="Z1" s="1">
-        <v>5.78703837E8</v>
+        <v>578703837</v>
       </c>
       <c r="AA1" s="1">
-        <v>5.78703841E8</v>
+        <v>578703841</v>
       </c>
       <c r="AB1" s="1">
-        <v>5.79960522E8</v>
+        <v>579960522</v>
       </c>
       <c r="AC1" s="1">
-        <v>6.28040069E8</v>
+        <v>628040069</v>
       </c>
       <c r="AD1" s="1">
-        <v>6.34379791E8</v>
+        <v>634379791</v>
       </c>
       <c r="AE1" s="1">
-        <v>6.49705832E8</v>
+        <v>649705832</v>
       </c>
       <c r="AF1" s="1">
-        <v>6.60855917E8</v>
+        <v>660855917</v>
       </c>
       <c r="AG1" s="1">
-        <v>7.41162914E8</v>
+        <v>741162914</v>
       </c>
       <c r="AH1" s="1">
-        <v>8.40623193E8</v>
+        <v>840623193</v>
       </c>
       <c r="AI1" s="1">
-        <v>8.53881923E8</v>
+        <v>853881923</v>
       </c>
       <c r="AJ1" s="1">
-        <v>8.58317954E8</v>
+        <v>858317954</v>
       </c>
       <c r="AK1" s="1">
-        <v>8.8876264E8</v>
+        <v>888762640</v>
       </c>
       <c r="AL1" s="1">
-        <v>8.91116578E8</v>
+        <v>891116578</v>
       </c>
       <c r="AM1" s="1">
-        <v>9.07134697E8</v>
+        <v>907134697</v>
       </c>
       <c r="AN1" s="1">
-        <v>9.0967453E8</v>
+        <v>909674530</v>
       </c>
       <c r="AO1" s="1">
-        <v>9.22756663E8</v>
+        <v>922756663</v>
       </c>
       <c r="AP1" s="1">
-        <v>9.41519793E8</v>
+        <v>941519793</v>
       </c>
       <c r="AQ1" s="1">
-        <v>9.53603864E8</v>
+        <v>953603864</v>
       </c>
       <c r="AR1" s="1">
-        <v>9.64467872E8</v>
+        <v>964467872</v>
       </c>
       <c r="AS1" s="1">
-        <v>9.72434583E8</v>
+        <v>972434583</v>
       </c>
       <c r="AT1" s="1">
-        <v>9.83415168E8</v>
+        <v>983415168</v>
       </c>
       <c r="AU1" s="1">
-        <v>1.033557392E9</v>
+        <v>1033557392</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>10326.0</v>
+        <v>103260</v>
       </c>
       <c r="C2" s="3">
-        <v>3754.0</v>
+        <v>37540</v>
       </c>
       <c r="D2" s="3">
-        <v>3608.0</v>
+        <v>36080</v>
       </c>
       <c r="E2" s="3">
-        <v>10601.0</v>
+        <v>106010</v>
       </c>
       <c r="F2" s="3">
-        <v>11796.0</v>
+        <v>117960</v>
       </c>
       <c r="G2" s="3">
-        <v>1885.0</v>
+        <v>18850</v>
       </c>
       <c r="H2" s="3">
-        <v>8152.0</v>
+        <v>81520</v>
       </c>
       <c r="I2" s="3">
-        <v>777.0</v>
+        <v>7770</v>
       </c>
       <c r="J2" s="3">
-        <v>4745.0</v>
+        <v>47450</v>
       </c>
       <c r="K2" s="3">
-        <v>3159.0</v>
+        <v>31590</v>
       </c>
       <c r="L2" s="3">
-        <v>3572.0</v>
+        <v>35720</v>
       </c>
       <c r="M2" s="3">
-        <v>3585.0</v>
+        <v>35850</v>
       </c>
       <c r="N2" s="3">
-        <v>1280.0</v>
+        <v>1280000</v>
       </c>
       <c r="O2" s="3">
-        <v>3018.0</v>
+        <v>30180</v>
       </c>
       <c r="P2" s="3">
-        <v>16526.0</v>
+        <v>165260</v>
       </c>
       <c r="Q2" s="3">
-        <v>1524.0</v>
+        <v>15240</v>
       </c>
       <c r="R2" s="3">
-        <v>9108.0</v>
+        <v>91080</v>
       </c>
       <c r="S2" s="3">
-        <v>35.0</v>
+        <v>350</v>
       </c>
       <c r="T2" s="3">
-        <v>7131.0</v>
+        <v>71310</v>
       </c>
       <c r="U2" s="3">
-        <v>14626.0</v>
+        <v>146260</v>
       </c>
       <c r="V2" s="3">
-        <v>5462.0</v>
+        <v>54620</v>
       </c>
       <c r="W2" s="3">
-        <v>15207.0</v>
+        <v>152070</v>
       </c>
       <c r="X2" s="3">
-        <v>3706.0</v>
+        <v>37060</v>
       </c>
       <c r="Y2" s="3">
-        <v>8.0</v>
+        <v>80</v>
       </c>
       <c r="Z2" s="3">
-        <v>475.0</v>
+        <v>4750</v>
       </c>
       <c r="AA2" s="3">
-        <v>7024.0</v>
+        <v>70240</v>
       </c>
       <c r="AB2" s="3">
-        <v>18405.0</v>
+        <v>184050</v>
       </c>
       <c r="AC2" s="3">
-        <v>10068.0</v>
+        <v>100680</v>
       </c>
       <c r="AD2" s="3">
-        <v>18041.0</v>
+        <v>180410</v>
       </c>
       <c r="AE2" s="3">
-        <v>15276.0</v>
+        <v>152760</v>
       </c>
       <c r="AF2" s="3">
-        <v>9101.0</v>
+        <v>91010</v>
       </c>
       <c r="AG2" s="3">
-        <v>19945.0</v>
+        <v>199450</v>
       </c>
       <c r="AH2" s="3">
-        <v>10074.0</v>
+        <v>100740</v>
       </c>
       <c r="AI2" s="3">
-        <v>17016.0</v>
+        <v>170160</v>
       </c>
       <c r="AJ2" s="3">
-        <v>19868.0</v>
+        <v>198680</v>
       </c>
       <c r="AK2" s="3">
-        <v>12168.0</v>
+        <v>121680</v>
       </c>
       <c r="AL2" s="3">
-        <v>13371.0</v>
+        <v>133710</v>
       </c>
       <c r="AM2" s="3">
-        <v>9314.0</v>
+        <v>93140</v>
       </c>
       <c r="AN2" s="3">
-        <v>13883.0</v>
+        <v>138830</v>
       </c>
       <c r="AO2" s="3">
-        <v>4723.0</v>
+        <v>47230</v>
       </c>
       <c r="AP2" s="3">
-        <v>4023.0</v>
+        <v>40230</v>
       </c>
       <c r="AQ2" s="3">
-        <v>16036.0</v>
+        <v>160360</v>
       </c>
       <c r="AR2" s="3">
-        <v>9663.0</v>
+        <v>96630</v>
       </c>
       <c r="AS2" s="3">
-        <v>8817.0</v>
+        <v>88170</v>
       </c>
       <c r="AT2" s="3">
-        <v>6501.0</v>
+        <v>65010</v>
       </c>
       <c r="AU2" s="3">
-        <v>8571.0</v>
+        <v>85710</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>13969.0</v>
+        <v>1396900</v>
       </c>
       <c r="C3" s="3">
-        <v>6285.0</v>
+        <v>628500</v>
       </c>
       <c r="D3" s="3">
-        <v>6695.0</v>
+        <v>669500</v>
       </c>
       <c r="E3" s="3">
-        <v>17959.0</v>
+        <v>1795900</v>
       </c>
       <c r="F3" s="3">
-        <v>12075.0</v>
+        <v>1207500</v>
       </c>
       <c r="G3" s="3">
-        <v>3709.0</v>
+        <v>370900</v>
       </c>
       <c r="H3" s="3">
-        <v>17049.0</v>
+        <v>1704900</v>
       </c>
       <c r="I3" s="3">
-        <v>2813.0</v>
+        <v>2813000</v>
       </c>
       <c r="J3" s="3">
-        <v>6695.0</v>
+        <v>6695000</v>
       </c>
       <c r="K3" s="3">
-        <v>3885.0</v>
+        <v>3885000</v>
       </c>
       <c r="L3" s="3">
-        <v>5597.0</v>
+        <v>5597000</v>
       </c>
       <c r="M3" s="3">
-        <v>19412.0</v>
+        <v>1941200</v>
       </c>
       <c r="N3" s="3">
-        <v>4429.0</v>
+        <v>4429000</v>
       </c>
       <c r="O3" s="3">
-        <v>13729.0</v>
+        <v>1372900</v>
       </c>
       <c r="P3" s="3">
-        <v>10822.0</v>
+        <v>1082200</v>
       </c>
       <c r="Q3" s="3">
-        <v>13811.0</v>
+        <v>1381100</v>
       </c>
       <c r="R3" s="3">
-        <v>342.0</v>
+        <v>34200</v>
       </c>
       <c r="S3" s="3">
-        <v>16959.0</v>
+        <v>1695900</v>
       </c>
       <c r="T3" s="3">
-        <v>3739.0</v>
+        <v>373900</v>
       </c>
       <c r="U3" s="3">
-        <v>782.0</v>
+        <v>78200</v>
       </c>
       <c r="V3" s="3">
-        <v>1335.0</v>
+        <v>133500</v>
       </c>
       <c r="W3" s="3">
-        <v>3416.0</v>
+        <v>341600</v>
       </c>
       <c r="X3" s="3">
-        <v>8561.0</v>
+        <v>856100</v>
       </c>
       <c r="Y3" s="3">
-        <v>740.0</v>
+        <v>74000</v>
       </c>
       <c r="Z3" s="3">
-        <v>11815.0</v>
+        <v>1181500</v>
       </c>
       <c r="AA3" s="3">
-        <v>9058.0</v>
+        <v>905800</v>
       </c>
       <c r="AB3" s="3">
-        <v>3046.0</v>
+        <v>304600</v>
       </c>
       <c r="AC3" s="3">
-        <v>7526.0</v>
+        <v>752600</v>
       </c>
       <c r="AD3" s="3">
-        <v>11078.0</v>
+        <v>1107800</v>
       </c>
       <c r="AE3" s="3">
-        <v>9985.0</v>
+        <v>998500</v>
       </c>
       <c r="AF3" s="3">
-        <v>12368.0</v>
+        <v>1236800</v>
       </c>
       <c r="AG3" s="3">
-        <v>3827.0</v>
+        <v>382700</v>
       </c>
       <c r="AH3" s="3">
-        <v>904.0</v>
+        <v>90400</v>
       </c>
       <c r="AI3" s="3">
-        <v>16118.0</v>
+        <v>1611800</v>
       </c>
       <c r="AJ3" s="3">
-        <v>13276.0</v>
+        <v>1327600</v>
       </c>
       <c r="AK3" s="3">
-        <v>3636.0</v>
+        <v>363600</v>
       </c>
       <c r="AL3" s="3">
-        <v>2211.0</v>
+        <v>221100</v>
       </c>
       <c r="AM3" s="3">
-        <v>14333.0</v>
+        <v>1433300</v>
       </c>
       <c r="AN3" s="3">
-        <v>11480.0</v>
+        <v>1148000</v>
       </c>
       <c r="AO3" s="3">
-        <v>16437.0</v>
+        <v>1643700</v>
       </c>
       <c r="AP3" s="3">
-        <v>13014.0</v>
+        <v>1301400</v>
       </c>
       <c r="AQ3" s="3">
-        <v>8468.0</v>
+        <v>846800</v>
       </c>
       <c r="AR3" s="3">
-        <v>19089.0</v>
+        <v>1908900</v>
       </c>
       <c r="AS3" s="3">
-        <v>15471.0</v>
+        <v>1547100</v>
       </c>
       <c r="AT3" s="3">
-        <v>8920.0</v>
+        <v>892000</v>
       </c>
       <c r="AU3" s="3">
-        <v>11307.0</v>
+        <v>1130700</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>1.4932E7</v>
+        <v>14932000</v>
       </c>
       <c r="C4" s="3">
-        <v>1.7094E7</v>
+        <v>17094000</v>
       </c>
       <c r="D4" s="3">
-        <v>1.7163E7</v>
+        <v>17163000</v>
       </c>
       <c r="E4" s="3">
-        <v>1.9155E7</v>
+        <v>19155000</v>
       </c>
       <c r="F4" s="3">
-        <v>1.2607E7</v>
+        <v>12607000</v>
       </c>
       <c r="G4" s="3">
-        <v>1.4503E7</v>
+        <v>14503000</v>
       </c>
       <c r="H4" s="3">
-        <v>1.7701E7</v>
+        <v>17701000</v>
       </c>
       <c r="I4" s="3">
-        <v>1.6796E7</v>
+        <v>16796000</v>
       </c>
       <c r="J4" s="3">
-        <v>1.2961E7</v>
+        <v>12961000</v>
       </c>
       <c r="K4" s="3">
-        <v>1.2602E7</v>
+        <v>12602000</v>
       </c>
       <c r="L4" s="3">
-        <v>1.5584E7</v>
+        <v>15584000</v>
       </c>
       <c r="M4" s="3">
-        <v>1.1714E7</v>
+        <v>11714000</v>
       </c>
       <c r="N4" s="3">
-        <v>1.168E7</v>
+        <v>11680000</v>
       </c>
       <c r="O4" s="3">
-        <v>1.8441E7</v>
+        <v>18441000</v>
       </c>
       <c r="P4" s="3">
-        <v>1.9188E7</v>
+        <v>19188000</v>
       </c>
       <c r="Q4" s="3">
-        <v>1.9485E7</v>
+        <v>19485000</v>
       </c>
       <c r="R4" s="3">
-        <v>1.0506E7</v>
+        <v>10506000</v>
       </c>
       <c r="S4" s="3">
-        <v>1.9636E7</v>
+        <v>19636000</v>
       </c>
       <c r="T4" s="3">
-        <v>1.9121E7</v>
+        <v>19121000</v>
       </c>
       <c r="U4" s="3">
-        <v>5444000.0</v>
+        <v>5444000</v>
       </c>
       <c r="V4" s="3">
-        <v>1.3848E7</v>
+        <v>13848000</v>
       </c>
       <c r="W4" s="3">
-        <v>1.2935E7</v>
+        <v>12935000</v>
       </c>
       <c r="X4" s="3">
-        <v>1.6528E7</v>
+        <v>16528000</v>
       </c>
       <c r="Y4" s="3">
-        <v>6838000.0</v>
+        <v>6838000</v>
       </c>
       <c r="Z4" s="3">
-        <v>9465000.0</v>
+        <v>9465000</v>
       </c>
       <c r="AA4" s="3">
-        <v>1.67E7</v>
+        <v>16700000</v>
       </c>
       <c r="AB4" s="3">
-        <v>1.0237E7</v>
+        <v>10237000</v>
       </c>
       <c r="AC4" s="3">
-        <v>5705000.0</v>
+        <v>5705000</v>
       </c>
       <c r="AD4" s="3">
-        <v>5581000.0</v>
+        <v>5581000</v>
       </c>
       <c r="AE4" s="3">
-        <v>5739000.0</v>
+        <v>5739000</v>
       </c>
       <c r="AF4" s="3">
-        <v>1640000.0</v>
+        <v>1640000</v>
       </c>
       <c r="AG4" s="3">
-        <v>9579000.0</v>
+        <v>9579000</v>
       </c>
       <c r="AH4" s="3">
-        <v>182000.0</v>
+        <v>182000</v>
       </c>
       <c r="AI4" s="3">
-        <v>1937000.0</v>
+        <v>1937000</v>
       </c>
       <c r="AJ4" s="3">
-        <v>1.175E7</v>
+        <v>11750000</v>
       </c>
       <c r="AK4" s="3">
-        <v>1.9064E7</v>
+        <v>19064000</v>
       </c>
       <c r="AL4" s="3">
-        <v>1.1249E7</v>
+        <v>11249000</v>
       </c>
       <c r="AM4" s="3">
-        <v>9743000.0</v>
+        <v>9743000</v>
       </c>
       <c r="AN4" s="3">
-        <v>824000.0</v>
+        <v>824000</v>
       </c>
       <c r="AO4" s="3">
-        <v>2633000.0</v>
+        <v>2633000</v>
       </c>
       <c r="AP4" s="3">
-        <v>1.268E7</v>
+        <v>12680000</v>
       </c>
       <c r="AQ4" s="3">
-        <v>1.9304E7</v>
+        <v>19304000</v>
       </c>
       <c r="AR4" s="3">
-        <v>1605000.0</v>
+        <v>1605000</v>
       </c>
       <c r="AS4" s="3">
-        <v>1.9516E7</v>
+        <v>19516000</v>
       </c>
       <c r="AT4" s="3">
-        <v>1.2795E7</v>
+        <v>12795000</v>
       </c>
       <c r="AU4" s="3">
-        <v>1.6908E7</v>
+        <v>16908000</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>